<commit_message>
fix: bug filter kategori
</commit_message>
<xml_diff>
--- a/Minggu-8/PWL_POS_JS8/public/template_barang.xlsx
+++ b/Minggu-8/PWL_POS_JS8/public/template_barang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_2025\Minggu-8\PWL_POS_JS8\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700F9E8F-22F4-4F7C-9785-7D365AAD109C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE026DA-0BB0-4141-BEC6-196A09F416D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26334BE9-E653-4BA8-AF8C-33395A51F8FD}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -481,7 +481,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>

</xml_diff>